<commit_message>
Actualizado con la n
</commit_message>
<xml_diff>
--- a/practica2/CalibrarVelocidades.xlsx
+++ b/practica2/CalibrarVelocidades.xlsx
@@ -206,6 +206,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -216,12 +222,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -405,11 +405,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103257984"/>
-        <c:axId val="103272448"/>
+        <c:axId val="87397888"/>
+        <c:axId val="87399808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103257984"/>
+        <c:axId val="87397888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,12 +466,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103272448"/>
+        <c:crossAx val="87399808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103272448"/>
+        <c:axId val="87399808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +528,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103257984"/>
+        <c:crossAx val="87397888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -744,11 +744,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="104664064"/>
-        <c:axId val="104690816"/>
+        <c:axId val="87952000"/>
+        <c:axId val="87974656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104664064"/>
+        <c:axId val="87952000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,12 +805,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104690816"/>
+        <c:crossAx val="87974656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104690816"/>
+        <c:axId val="87974656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,7 +867,672 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104664064"/>
+        <c:crossAx val="87952000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MOTOR A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.640608111111111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3423026944444443</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0876304722222221</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8067783333333329</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5346528333333325</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.253800694444445</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.972948555555556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="10989568"/>
+        <c:axId val="10991488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="10989568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10991488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="10991488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10989568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MOTOR B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$H$3:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.64933475</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3772092499999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0876304722222221</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8155049722222216</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.543379472222222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.253800694444445</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.972948555555556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="11739520"/>
+        <c:axId val="11741440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="11739520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11741440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="11741440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11739520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -973,6 +1638,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Gráfico 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1236,7 +1965,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1246,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1256,20 +1985,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1496,10 +2225,10 @@
         <f t="shared" si="5"/>
         <v>0.17038762430555554</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="11"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1578,10 +2307,10 @@
         <f t="shared" si="5"/>
         <v>0.17089667824074076</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="12"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1620,11 +2349,11 @@
         <f t="shared" si="5"/>
         <v>0.17104212222222223</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="9">
         <f>SLOPE(A3:A9,G3:G9)</f>
         <v>5.8010345394965368</v>
       </c>
-      <c r="N9" s="13"/>
+      <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1663,10 +2392,10 @@
         <f t="shared" si="5"/>
         <v>0.15315251249999998</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="12"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1705,11 +2434,11 @@
         <f t="shared" si="5"/>
         <v>0.13603860401234569</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="9">
         <f>SLOPE(B3:B9,H3:H9)</f>
         <v>5.8115569162125311</v>
       </c>
-      <c r="N11" s="13"/>
+      <c r="N11" s="9"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">

</xml_diff>